<commit_message>
Correzione colonna backoffici per casi di test 158 168
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/dedalus/caleido_fse20_connector/2023/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/dedalus/caleido_fse20_connector/2023/accreditamento-checklist_V8.1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/lucia_trama_dedalus_eu/Documents/Documenti/PROGETTI/FSE/2.0/accreditamento/FASE 1/FASE 1 LAB-RAD-RSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="613" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4334F8ED-6725-4D01-9952-383EB0271B3A}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93198BEF-0867-4C03-A3E2-4B1F29314B3D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="363" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4595,10 +4595,10 @@
   <dimension ref="A1:T660"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="Q82" sqref="Q82"/>
+      <selection pane="bottomRight" activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -5911,7 +5911,7 @@
         <v>275</v>
       </c>
       <c r="O33" s="24" t="s">
-        <v>259</v>
+        <v>87</v>
       </c>
       <c r="P33" s="24" t="s">
         <v>276</v>
@@ -5965,7 +5965,7 @@
         <v>275</v>
       </c>
       <c r="O34" s="24" t="s">
-        <v>259</v>
+        <v>87</v>
       </c>
       <c r="P34" s="24" t="s">
         <v>288</v>
@@ -7405,7 +7405,7 @@
         <v>275</v>
       </c>
       <c r="O69" s="24" t="s">
-        <v>259</v>
+        <v>87</v>
       </c>
       <c r="P69" s="24" t="s">
         <v>363</v>
@@ -7801,7 +7801,7 @@
         <v>275</v>
       </c>
       <c r="O79" s="24" t="s">
-        <v>259</v>
+        <v>87</v>
       </c>
       <c r="P79" s="24" t="s">
         <v>364</v>

</xml_diff>